<commit_message>
Actualização de ficheiros com Tarefas
</commit_message>
<xml_diff>
--- a/6_Organiçao de Grupo (Importante)/Tarefas_app.xlsx
+++ b/6_Organiçao de Grupo (Importante)/Tarefas_app.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Folha2" sheetId="2" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -733,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -810,6 +810,158 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -822,15 +974,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -840,158 +983,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,7 +1053,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1087,7 +1088,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1298,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:D30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,11 +1316,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1391,11 +1392,11 @@
       <c r="A9" s="18">
         <v>1</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="66"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="87"/>
       <c r="E9" s="14" t="s">
         <v>2</v>
       </c>
@@ -1412,12 +1413,12 @@
         <f>A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="94"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="62" t="s">
+      <c r="C10" s="83"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="114" t="s">
         <v>64</v>
       </c>
       <c r="F10" s="24" t="s">
@@ -1426,7 +1427,7 @@
       <c r="G10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="60" t="s">
+      <c r="H10" s="112" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1435,30 +1436,30 @@
         <f t="shared" ref="A11:A73" si="0">A10+1</f>
         <v>3</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="63"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="115"/>
       <c r="F11" s="24" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="61"/>
+      <c r="H11" s="113"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="65"/>
-      <c r="D12" s="66"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="87"/>
       <c r="E12" s="12" t="s">
         <v>27</v>
       </c>
@@ -1475,11 +1476,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="66"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="87"/>
       <c r="E13" s="14" t="s">
         <v>2</v>
       </c>
@@ -1496,11 +1497,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B14" s="105" t="s">
+      <c r="B14" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="106"/>
-      <c r="D14" s="107"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="99"/>
       <c r="E14" s="14" t="s">
         <v>2</v>
       </c>
@@ -1517,11 +1518,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="101"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="93"/>
       <c r="E15" s="16" t="s">
         <v>6</v>
       </c>
@@ -1538,11 +1539,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="66"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="14" t="s">
         <v>5</v>
       </c>
@@ -1559,11 +1560,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="87"/>
       <c r="E17" s="14" t="s">
         <v>5</v>
       </c>
@@ -1580,11 +1581,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="83"/>
-      <c r="D18" s="84"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="16" t="s">
         <v>7</v>
       </c>
@@ -1601,11 +1602,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="102" t="s">
+      <c r="B19" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="103"/>
-      <c r="D19" s="104"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="96"/>
       <c r="E19" s="19" t="s">
         <v>2</v>
       </c>
@@ -1622,11 +1623,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="87"/>
       <c r="E20" s="12" t="s">
         <v>5</v>
       </c>
@@ -1643,11 +1644,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="101"/>
+      <c r="D21" s="102"/>
       <c r="E21" s="7"/>
       <c r="F21" s="27"/>
       <c r="G21" s="29"/>
@@ -1658,11 +1659,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="87"/>
       <c r="E22" s="15" t="s">
         <v>5</v>
       </c>
@@ -1681,11 +1682,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="87"/>
       <c r="E23" s="12" t="s">
         <v>27</v>
       </c>
@@ -1702,12 +1703,12 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B24" s="118" t="s">
+      <c r="B24" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="119"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="121"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="61"/>
       <c r="F24" s="28" t="s">
         <v>14</v>
       </c>
@@ -1721,11 +1722,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="87"/>
       <c r="E25" s="15" t="s">
         <v>2</v>
       </c>
@@ -1742,11 +1743,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="86"/>
-      <c r="D26" s="87"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="111"/>
       <c r="E26" s="44" t="s">
         <v>27</v>
       </c>
@@ -1763,11 +1764,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B27" s="96" t="s">
+      <c r="B27" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="97"/>
-      <c r="D27" s="98"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="90"/>
       <c r="E27" s="48" t="s">
         <v>27</v>
       </c>
@@ -1826,9 +1827,9 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="78"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="79"/>
       <c r="E30" s="7"/>
       <c r="F30" s="27"/>
       <c r="G30" s="29"/>
@@ -1839,11 +1840,11 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B31" s="70" t="s">
+      <c r="B31" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="72"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="102"/>
       <c r="E31" s="7"/>
       <c r="F31" s="27"/>
       <c r="G31" s="29"/>
@@ -1854,11 +1855,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B32" s="88" t="s">
+      <c r="B32" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="89"/>
-      <c r="D32" s="90"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="64"/>
       <c r="E32" s="16" t="s">
         <v>69</v>
       </c>
@@ -1875,11 +1876,11 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B33" s="88" t="s">
+      <c r="B33" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="90"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="64"/>
       <c r="E33" s="16" t="s">
         <v>69</v>
       </c>
@@ -1896,11 +1897,11 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B34" s="88" t="s">
+      <c r="B34" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="89"/>
-      <c r="D34" s="90"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="64"/>
       <c r="E34" s="40" t="s">
         <v>5</v>
       </c>
@@ -1917,11 +1918,11 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="89"/>
-      <c r="D35" s="90"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="64"/>
       <c r="E35" s="40" t="s">
         <v>5</v>
       </c>
@@ -1938,11 +1939,11 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B36" s="88" t="s">
+      <c r="B36" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="89"/>
-      <c r="D36" s="90"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="64"/>
       <c r="E36" s="55" t="s">
         <v>3</v>
       </c>
@@ -1959,11 +1960,11 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B37" s="88" t="s">
+      <c r="B37" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="89"/>
-      <c r="D37" s="90"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="64"/>
       <c r="E37" s="55" t="s">
         <v>3</v>
       </c>
@@ -1980,11 +1981,11 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B38" s="88" t="s">
+      <c r="B38" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="89"/>
-      <c r="D38" s="90"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="64"/>
       <c r="E38" s="55" t="s">
         <v>7</v>
       </c>
@@ -2001,11 +2002,11 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B39" s="88" t="s">
+      <c r="B39" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="89"/>
-      <c r="D39" s="90"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="64"/>
       <c r="E39" s="55" t="s">
         <v>7</v>
       </c>
@@ -2022,9 +2023,9 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B40" s="108"/>
-      <c r="C40" s="109"/>
-      <c r="D40" s="110"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="75"/>
+      <c r="D40" s="76"/>
       <c r="E40" s="8"/>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
@@ -2035,11 +2036,11 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="77"/>
-      <c r="D41" s="78"/>
+      <c r="C41" s="78"/>
+      <c r="D41" s="79"/>
       <c r="E41" s="8"/>
       <c r="F41" s="28" t="s">
         <v>14</v>
@@ -2054,9 +2055,9 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B42" s="76"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="78"/>
+      <c r="B42" s="77"/>
+      <c r="C42" s="78"/>
+      <c r="D42" s="79"/>
       <c r="E42" s="8"/>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
@@ -2067,9 +2068,9 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B43" s="79"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="81"/>
+      <c r="B43" s="106"/>
+      <c r="C43" s="107"/>
+      <c r="D43" s="108"/>
       <c r="E43" s="7"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
@@ -2080,12 +2081,12 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B44" s="118" t="s">
+      <c r="B44" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="119"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="121"/>
+      <c r="C44" s="104"/>
+      <c r="D44" s="105"/>
+      <c r="E44" s="61"/>
       <c r="F44" s="28" t="s">
         <v>14</v>
       </c>
@@ -2099,11 +2100,11 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="71"/>
-      <c r="D45" s="72"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="102"/>
       <c r="E45" s="7"/>
       <c r="F45" s="27"/>
       <c r="G45" s="29"/>
@@ -2114,11 +2115,11 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="65"/>
-      <c r="D46" s="66"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="87"/>
       <c r="E46" s="15" t="s">
         <v>5</v>
       </c>
@@ -2135,9 +2136,9 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B47" s="108"/>
-      <c r="C47" s="109"/>
-      <c r="D47" s="110"/>
+      <c r="B47" s="74"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="76"/>
       <c r="E47" s="13"/>
       <c r="F47" s="30"/>
       <c r="G47" s="36"/>
@@ -2148,9 +2149,9 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B48" s="108"/>
-      <c r="C48" s="109"/>
-      <c r="D48" s="110"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="75"/>
+      <c r="D48" s="76"/>
       <c r="E48" s="13"/>
       <c r="F48" s="30"/>
       <c r="G48" s="36"/>
@@ -2161,9 +2162,9 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B49" s="108"/>
-      <c r="C49" s="109"/>
-      <c r="D49" s="110"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="76"/>
       <c r="E49" s="13"/>
       <c r="F49" s="30"/>
       <c r="G49" s="36"/>
@@ -2174,9 +2175,9 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B50" s="108"/>
-      <c r="C50" s="109"/>
-      <c r="D50" s="110"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="76"/>
       <c r="E50" s="13"/>
       <c r="F50" s="30"/>
       <c r="G50" s="36"/>
@@ -2187,11 +2188,11 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B51" s="64" t="s">
+      <c r="B51" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="65"/>
-      <c r="D51" s="66"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="87"/>
       <c r="E51" s="12" t="s">
         <v>2</v>
       </c>
@@ -2208,11 +2209,11 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B52" s="64" t="s">
+      <c r="B52" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="65"/>
-      <c r="D52" s="66"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="87"/>
       <c r="E52" s="14" t="s">
         <v>5</v>
       </c>
@@ -2231,9 +2232,9 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B53" s="73"/>
-      <c r="C53" s="74"/>
-      <c r="D53" s="75"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="73"/>
       <c r="E53" s="8"/>
       <c r="F53" s="29"/>
       <c r="G53" s="29"/>
@@ -2244,12 +2245,12 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B54" s="111" t="s">
+      <c r="B54" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="112"/>
-      <c r="D54" s="113"/>
-      <c r="E54" s="114"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="70"/>
+      <c r="E54" s="60"/>
       <c r="F54" s="28" t="s">
         <v>14</v>
       </c>
@@ -2263,12 +2264,12 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B55" s="111" t="s">
+      <c r="B55" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="112"/>
-      <c r="D55" s="113"/>
-      <c r="E55" s="114"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="28" t="s">
         <v>14</v>
       </c>
@@ -2282,33 +2283,33 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B56" s="115" t="s">
+      <c r="B56" s="119" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="116"/>
-      <c r="D56" s="117"/>
-      <c r="E56" s="55" t="s">
+      <c r="C56" s="120"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="F56" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G56" s="37" t="s">
+      <c r="F56" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="H56" s="10"/>
+      <c r="H56" s="122"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="18">
         <f t="shared" ref="A57:A59" si="1">A53+1</f>
         <v>46</v>
       </c>
-      <c r="B57" s="111" t="s">
+      <c r="B57" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="112"/>
-      <c r="D57" s="113"/>
-      <c r="E57" s="114"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="70"/>
+      <c r="E57" s="60"/>
       <c r="F57" s="28" t="s">
         <v>14</v>
       </c>
@@ -2322,33 +2323,33 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B58" s="115" t="s">
+      <c r="B58" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="C58" s="116"/>
-      <c r="D58" s="117"/>
-      <c r="E58" s="55" t="s">
+      <c r="C58" s="120"/>
+      <c r="D58" s="121"/>
+      <c r="E58" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F58" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G58" s="37" t="s">
+      <c r="F58" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="H58" s="10"/>
+      <c r="H58" s="122"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B59" s="111" t="s">
+      <c r="B59" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="C59" s="112"/>
-      <c r="D59" s="113"/>
-      <c r="E59" s="114"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="70"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="28" t="s">
         <v>14</v>
       </c>
@@ -2362,12 +2363,12 @@
         <f>A56+1</f>
         <v>49</v>
       </c>
-      <c r="B60" s="111" t="s">
+      <c r="B60" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="112"/>
-      <c r="D60" s="113"/>
-      <c r="E60" s="114"/>
+      <c r="C60" s="69"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="28" t="s">
         <v>14</v>
       </c>
@@ -2381,9 +2382,9 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B61" s="73"/>
-      <c r="C61" s="74"/>
-      <c r="D61" s="75"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="72"/>
+      <c r="D61" s="73"/>
       <c r="E61" s="8"/>
       <c r="F61" s="29"/>
       <c r="G61" s="29"/>
@@ -2394,11 +2395,11 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B62" s="73" t="s">
+      <c r="B62" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="74"/>
-      <c r="D62" s="75"/>
+      <c r="C62" s="72"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="8"/>
       <c r="F62" s="29"/>
       <c r="G62" s="29" t="s">
@@ -2411,11 +2412,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B63" s="64" t="s">
+      <c r="B63" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C63" s="65"/>
-      <c r="D63" s="66"/>
+      <c r="C63" s="86"/>
+      <c r="D63" s="87"/>
       <c r="E63" s="15" t="s">
         <v>2</v>
       </c>
@@ -2432,11 +2433,11 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B64" s="82" t="s">
+      <c r="B64" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="83"/>
-      <c r="D64" s="84"/>
+      <c r="C64" s="66"/>
+      <c r="D64" s="67"/>
       <c r="E64" s="55" t="s">
         <v>2</v>
       </c>
@@ -2453,11 +2454,11 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B65" s="64" t="s">
+      <c r="B65" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C65" s="65"/>
-      <c r="D65" s="66"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="87"/>
       <c r="E65" s="56" t="s">
         <v>2</v>
       </c>
@@ -2474,11 +2475,11 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B66" s="64" t="s">
+      <c r="B66" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="C66" s="65"/>
-      <c r="D66" s="66"/>
+      <c r="C66" s="86"/>
+      <c r="D66" s="87"/>
       <c r="E66" s="56" t="s">
         <v>2</v>
       </c>
@@ -2495,11 +2496,11 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B67" s="64" t="s">
+      <c r="B67" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="65"/>
-      <c r="D67" s="66"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="87"/>
       <c r="E67" s="56" t="s">
         <v>2</v>
       </c>
@@ -2516,11 +2517,11 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B68" s="64" t="s">
+      <c r="B68" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="C68" s="65"/>
-      <c r="D68" s="66"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="87"/>
       <c r="E68" s="56" t="s">
         <v>2</v>
       </c>
@@ -2539,11 +2540,11 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B69" s="64" t="s">
+      <c r="B69" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="C69" s="65"/>
-      <c r="D69" s="66"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="87"/>
       <c r="E69" s="56" t="s">
         <v>2</v>
       </c>
@@ -2560,9 +2561,9 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B70" s="76"/>
-      <c r="C70" s="77"/>
-      <c r="D70" s="78"/>
+      <c r="B70" s="77"/>
+      <c r="C70" s="78"/>
+      <c r="D70" s="79"/>
       <c r="E70" s="8"/>
       <c r="F70" s="29"/>
       <c r="G70" s="29"/>
@@ -2573,9 +2574,9 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B71" s="76"/>
-      <c r="C71" s="77"/>
-      <c r="D71" s="78"/>
+      <c r="B71" s="77"/>
+      <c r="C71" s="78"/>
+      <c r="D71" s="79"/>
       <c r="E71" s="8"/>
       <c r="F71" s="29"/>
       <c r="G71" s="29"/>
@@ -2586,11 +2587,11 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B72" s="76" t="s">
+      <c r="B72" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C72" s="77"/>
-      <c r="D72" s="78"/>
+      <c r="C72" s="78"/>
+      <c r="D72" s="79"/>
       <c r="E72" s="13"/>
       <c r="F72" s="28" t="s">
         <v>14</v>
@@ -2607,9 +2608,9 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B73" s="67"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="69"/>
+      <c r="B73" s="116"/>
+      <c r="C73" s="117"/>
+      <c r="D73" s="118"/>
       <c r="E73" s="9"/>
       <c r="F73" s="31"/>
       <c r="G73" s="31"/>
@@ -2617,24 +2618,38 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B38:D38"/>
@@ -2651,38 +2666,24 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>